<commit_message>
created a function for show password and terms and condition chkbox
</commit_message>
<xml_diff>
--- a/user_account_data.xlsx
+++ b/user_account_data.xlsx
@@ -417,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -540,6 +540,87 @@
         </is>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>awd</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>awd</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>awd</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>awd</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>awd</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>awd</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>awd</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>sss</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>sss</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>www</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>we</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>awe</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>wef</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>wef</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>ser</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
fixed the undeeded lines and added a few features to the portal
</commit_message>
<xml_diff>
--- a/user_account_data.xlsx
+++ b/user_account_data.xlsx
@@ -417,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -513,6 +513,87 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>ara</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>wr</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>ara@gmail.com</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>hfg</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>asdfgh</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>arw</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>wer</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>wer@gmail.com</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>awed</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>1111111</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>awr</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>wer</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>a@gmail.com</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>fda</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>ararara</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
added openpyxl in enrollment form, unfinished but has a starting progress
</commit_message>
<xml_diff>
--- a/user_account_data.xlsx
+++ b/user_account_data.xlsx
@@ -8,6 +8,9 @@
   </bookViews>
   <sheets>
     <sheet name="Userdata" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="1B Enrollment Information " sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="1A Enrollment Information " sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="1C Enrollment Information " sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -417,7 +420,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -462,56 +465,622 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>admin</t>
+          <t>awr</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>admin</t>
+          <t>awr</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>admin@gmail.com</t>
+          <t>dsa@gmail.com</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>admins</t>
+          <t>122</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>admin123</t>
+          <t>aqwaqw</t>
         </is>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>admins</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>admins</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>admins@gmail.com</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>admin</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>admin12</t>
-        </is>
-      </c>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:Z2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Student ID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Course/Section</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>LRN</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Surname</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Firstname</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Middle Initial</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>Gender</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>Age</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>Birthdate</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>Birthplace</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>Nationality</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>Religion</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>Marital Status</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>Language Spoken</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>Street</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>Barangay</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>City</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>Zip Code</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>Province</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>Country</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>Contact Number</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>awef</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>1B</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>awef</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>awef</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>awef</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>awef</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Prefer not to answer</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>29</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>January 17, 1930</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>aewf</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>awef</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>Iglesia ni Cristo</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>Single</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>awef</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>awfe</t>
+        </is>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>awe</t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>fwe</t>
+        </is>
+      </c>
+      <c r="U2" t="inlineStr">
+        <is>
+          <t>awe</t>
+        </is>
+      </c>
+      <c r="V2" t="inlineStr">
+        <is>
+          <t>wef</t>
+        </is>
+      </c>
+      <c r="W2" t="inlineStr">
+        <is>
+          <t>fwe</t>
+        </is>
+      </c>
+      <c r="Y2" t="inlineStr">
+        <is>
+          <t>wef</t>
+        </is>
+      </c>
+      <c r="Z2" t="inlineStr">
+        <is>
+          <t>fwe</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:Z2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Student ID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Course/Section</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>LRN</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Surname</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Firstname</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Middle Initial</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>Gender</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>Age</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>Birthdate</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>Birthplace</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>Nationality</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>Religion</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>Marital Status</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>Language Spoken</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>Street</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>Barangay</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>City</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>Zip Code</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>Province</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>Country</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>Contact Number</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>1A</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Prefer not to answer</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>Select Age</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>MM DD, YYYY</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>Select Religion</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>Select Marital Status</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:Z2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Student ID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Course/Section</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>LRN</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr"/>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Surname</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Firstname</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Middle Initial</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr"/>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>Gender</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>Age</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>Birthdate</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>Birthplace</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>Nationality</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>Religion</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>Marital Status</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>Language Spoken</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr"/>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>Street</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>Barangay</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>City</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>Zip Code</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>Province</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>Country</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr"/>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>Contact Number</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr"/>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>1C</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Prefer not to answer</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>Select Age</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>MM DD, YYYY</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr"/>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>Select Religion</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>Select Marital Status</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr"/>
+      <c r="Q2" t="inlineStr"/>
+      <c r="R2" t="inlineStr"/>
+      <c r="S2" t="inlineStr"/>
+      <c r="T2" t="inlineStr"/>
+      <c r="U2" t="inlineStr"/>
+      <c r="V2" t="inlineStr"/>
+      <c r="W2" t="inlineStr"/>
+      <c r="X2" t="inlineStr"/>
+      <c r="Y2" t="inlineStr"/>
+      <c r="Z2" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
new files and new changes
</commit_message>
<xml_diff>
--- a/user_account_data.xlsx
+++ b/user_account_data.xlsx
@@ -418,7 +418,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -484,6 +484,33 @@
       <c r="E2" t="inlineStr">
         <is>
           <t>admins</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>admins@gmail.com</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>admin123</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
done with admin panels just need some revisions
</commit_message>
<xml_diff>
--- a/user_account_data.xlsx
+++ b/user_account_data.xlsx
@@ -8,6 +8,8 @@
   </bookViews>
   <sheets>
     <sheet name="Userdata" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="1A Enrollment Information " sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="1B Enrollment Information " sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -417,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -462,54 +464,1071 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>admin</t>
+          <t>jok</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>admin</t>
+          <t>jok</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>admin@gmail.com</t>
+          <t>jok@gmail.com</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>admin</t>
+          <t>joke</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>admin123</t>
+          <t>jokjok</t>
         </is>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>joe</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>eoj</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>ejo@gmail.com</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>joey</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>123456</t>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AU2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="12" customWidth="1" min="1" max="1"/>
+    <col width="16" customWidth="1" min="2" max="2"/>
+    <col width="10" customWidth="1" min="3" max="3"/>
+    <col width="9" customWidth="1" min="4" max="4"/>
+    <col width="11" customWidth="1" min="5" max="5"/>
+    <col width="16" customWidth="1" min="6" max="6"/>
+    <col width="8" customWidth="1" min="7" max="7"/>
+    <col width="5" customWidth="1" min="8" max="8"/>
+    <col width="20" customWidth="1" min="9" max="9"/>
+    <col width="12" customWidth="1" min="10" max="10"/>
+    <col width="13" customWidth="1" min="11" max="11"/>
+    <col width="19" customWidth="1" min="12" max="12"/>
+    <col width="16" customWidth="1" min="13" max="13"/>
+    <col width="17" customWidth="1" min="14" max="14"/>
+    <col width="8" customWidth="1" min="15" max="15"/>
+    <col width="10" customWidth="1" min="16" max="16"/>
+    <col width="7" customWidth="1" min="17" max="17"/>
+    <col width="10" customWidth="1" min="18" max="18"/>
+    <col width="10" customWidth="1" min="19" max="19"/>
+    <col width="10" customWidth="1" min="20" max="20"/>
+    <col width="15" customWidth="1" min="21" max="21"/>
+    <col width="16" customWidth="1" min="22" max="22"/>
+    <col width="15" customWidth="1" min="23" max="23"/>
+    <col width="21" customWidth="1" min="24" max="24"/>
+    <col width="21" customWidth="1" min="25" max="25"/>
+    <col width="15" customWidth="1" min="26" max="26"/>
+    <col width="21" customWidth="1" min="27" max="27"/>
+    <col width="21" customWidth="1" min="28" max="28"/>
+    <col width="17" customWidth="1" min="29" max="29"/>
+    <col width="25" customWidth="1" min="30" max="30"/>
+    <col width="20" customWidth="1" min="31" max="31"/>
+    <col width="23" customWidth="1" min="32" max="32"/>
+    <col width="23" customWidth="1" min="33" max="33"/>
+    <col width="19" customWidth="1" min="34" max="34"/>
+    <col width="20" customWidth="1" min="35" max="35"/>
+    <col width="27" customWidth="1" min="36" max="36"/>
+    <col width="20" customWidth="1" min="37" max="37"/>
+    <col width="21" customWidth="1" min="38" max="38"/>
+    <col width="28" customWidth="1" min="39" max="39"/>
+    <col width="20" customWidth="1" min="40" max="40"/>
+    <col width="21" customWidth="1" min="41" max="41"/>
+    <col width="20" customWidth="1" min="42" max="42"/>
+    <col width="28" customWidth="1" min="43" max="43"/>
+    <col width="9" customWidth="1" min="44" max="44"/>
+    <col width="17" customWidth="1" min="45" max="45"/>
+    <col width="24" customWidth="1" min="46" max="46"/>
+    <col width="16" customWidth="1" min="47" max="47"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Student ID</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Course/Section</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>LRN</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Surname</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Firstname</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Middle Initial</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Gender</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Age</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Birthdate</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Birthplace</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Nationality</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Religion</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Marital Status</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Language Spoken</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Street</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Barangay</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>City</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>Zip Code</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>Province</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>Country</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>Contact Number</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>Father's Name</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>Father's Occupation</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>Father's Contact No</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>Mother's Name</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>Mother's Occupation</t>
+        </is>
+      </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>Mother's Contact No</t>
+        </is>
+      </c>
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
+          <t>Guardian's Name</t>
+        </is>
+      </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>Guardian's Relationship</t>
+        </is>
+      </c>
+      <c r="AE1" s="1" t="inlineStr">
+        <is>
+          <t>Guardian's Address</t>
+        </is>
+      </c>
+      <c r="AF1" s="1" t="inlineStr">
+        <is>
+          <t>Guardian's Occupation</t>
+        </is>
+      </c>
+      <c r="AG1" s="1" t="inlineStr">
+        <is>
+          <t>Guardian's Contact No</t>
+        </is>
+      </c>
+      <c r="AH1" s="1" t="inlineStr">
+        <is>
+          <t>Elementary School</t>
+        </is>
+      </c>
+      <c r="AI1" s="1" t="inlineStr">
+        <is>
+          <t>Elementary Address</t>
+        </is>
+      </c>
+      <c r="AJ1" s="1" t="inlineStr">
+        <is>
+          <t>Elementary Year Graduated</t>
+        </is>
+      </c>
+      <c r="AK1" s="1" t="inlineStr">
+        <is>
+          <t>Junior High School</t>
+        </is>
+      </c>
+      <c r="AL1" s="1" t="inlineStr">
+        <is>
+          <t>Junior High Address</t>
+        </is>
+      </c>
+      <c r="AM1" s="1" t="inlineStr">
+        <is>
+          <t>Junior High Year Graduated</t>
+        </is>
+      </c>
+      <c r="AN1" s="1" t="inlineStr">
+        <is>
+          <t>Senior High School</t>
+        </is>
+      </c>
+      <c r="AO1" s="1" t="inlineStr">
+        <is>
+          <t>Senior High Address</t>
+        </is>
+      </c>
+      <c r="AP1" s="1" t="inlineStr">
+        <is>
+          <t>Senior High Strand</t>
+        </is>
+      </c>
+      <c r="AQ1" s="1" t="inlineStr">
+        <is>
+          <t>Senior High Year Graduated</t>
+        </is>
+      </c>
+      <c r="AR1" s="1" t="inlineStr">
+        <is>
+          <t>College</t>
+        </is>
+      </c>
+      <c r="AS1" s="1" t="inlineStr">
+        <is>
+          <t>College Address</t>
+        </is>
+      </c>
+      <c r="AT1" s="1" t="inlineStr">
+        <is>
+          <t>College Year Graduated</t>
+        </is>
+      </c>
+      <c r="AU1" s="1" t="inlineStr">
+        <is>
+          <t>Student Status</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>123123</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>1A</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>12312312</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>jok</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>jok</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>awefwfe</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>33</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>September 21, 1935</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>awfwaef</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>waefawef</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>Iglesia ni Cristo</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>Single</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>awfeweafew</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>awfwe</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>awefwef</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>awfew</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>2124</t>
+        </is>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>awfeew</t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>awefweaf</t>
+        </is>
+      </c>
+      <c r="U2" t="inlineStr">
+        <is>
+          <t>jok@gmail.com</t>
+        </is>
+      </c>
+      <c r="V2" t="inlineStr">
+        <is>
+          <t>213213</t>
+        </is>
+      </c>
+      <c r="W2" t="inlineStr">
+        <is>
+          <t>awfe</t>
+        </is>
+      </c>
+      <c r="X2" t="inlineStr">
+        <is>
+          <t>fawef</t>
+        </is>
+      </c>
+      <c r="Y2" t="inlineStr">
+        <is>
+          <t>123123</t>
+        </is>
+      </c>
+      <c r="Z2" t="inlineStr">
+        <is>
+          <t>ewfawef</t>
+        </is>
+      </c>
+      <c r="AA2" t="inlineStr">
+        <is>
+          <t>awefwae</t>
+        </is>
+      </c>
+      <c r="AB2" t="inlineStr">
+        <is>
+          <t>123123</t>
+        </is>
+      </c>
+      <c r="AH2" t="inlineStr">
+        <is>
+          <t>awfwe</t>
+        </is>
+      </c>
+      <c r="AI2" t="inlineStr">
+        <is>
+          <t>fwaefewfawef</t>
+        </is>
+      </c>
+      <c r="AJ2" t="inlineStr">
+        <is>
+          <t>123123</t>
+        </is>
+      </c>
+      <c r="AK2" t="inlineStr">
+        <is>
+          <t>awerv</t>
+        </is>
+      </c>
+      <c r="AL2" t="inlineStr">
+        <is>
+          <t>awerv</t>
+        </is>
+      </c>
+      <c r="AM2" t="inlineStr">
+        <is>
+          <t>12312</t>
+        </is>
+      </c>
+      <c r="AN2" t="inlineStr">
+        <is>
+          <t>awefawef</t>
+        </is>
+      </c>
+      <c r="AO2" t="inlineStr">
+        <is>
+          <t>awefawef</t>
+        </is>
+      </c>
+      <c r="AP2" t="inlineStr">
+        <is>
+          <t>awefawef</t>
+        </is>
+      </c>
+      <c r="AQ2" t="inlineStr">
+        <is>
+          <t>123123</t>
+        </is>
+      </c>
+      <c r="AR2" t="inlineStr">
+        <is>
+          <t>awev</t>
+        </is>
+      </c>
+      <c r="AS2" t="inlineStr">
+        <is>
+          <t>awevr</t>
+        </is>
+      </c>
+      <c r="AT2" t="inlineStr">
+        <is>
+          <t>123123</t>
+        </is>
+      </c>
+      <c r="AU2" t="inlineStr">
+        <is>
+          <t>New Student</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:BE2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="12" customWidth="1" min="1" max="1"/>
+    <col width="16" customWidth="1" min="2" max="2"/>
+    <col width="8" customWidth="1" min="3" max="3"/>
+    <col width="2" customWidth="1" min="4" max="4"/>
+    <col width="9" customWidth="1" min="5" max="5"/>
+    <col width="11" customWidth="1" min="6" max="6"/>
+    <col width="16" customWidth="1" min="7" max="7"/>
+    <col width="2" customWidth="1" min="8" max="8"/>
+    <col width="8" customWidth="1" min="9" max="9"/>
+    <col width="5" customWidth="1" min="10" max="10"/>
+    <col width="15" customWidth="1" min="11" max="11"/>
+    <col width="12" customWidth="1" min="12" max="12"/>
+    <col width="13" customWidth="1" min="13" max="13"/>
+    <col width="12" customWidth="1" min="14" max="14"/>
+    <col width="16" customWidth="1" min="15" max="15"/>
+    <col width="17" customWidth="1" min="16" max="16"/>
+    <col width="2" customWidth="1" min="17" max="17"/>
+    <col width="8" customWidth="1" min="18" max="18"/>
+    <col width="10" customWidth="1" min="19" max="19"/>
+    <col width="7" customWidth="1" min="20" max="20"/>
+    <col width="10" customWidth="1" min="21" max="21"/>
+    <col width="10" customWidth="1" min="22" max="22"/>
+    <col width="9" customWidth="1" min="23" max="23"/>
+    <col width="2" customWidth="1" min="24" max="24"/>
+    <col width="15" customWidth="1" min="25" max="25"/>
+    <col width="16" customWidth="1" min="26" max="26"/>
+    <col width="2" customWidth="1" min="27" max="27"/>
+    <col width="15" customWidth="1" min="28" max="28"/>
+    <col width="21" customWidth="1" min="29" max="29"/>
+    <col width="21" customWidth="1" min="30" max="30"/>
+    <col width="15" customWidth="1" min="31" max="31"/>
+    <col width="21" customWidth="1" min="32" max="32"/>
+    <col width="21" customWidth="1" min="33" max="33"/>
+    <col width="2" customWidth="1" min="34" max="34"/>
+    <col width="17" customWidth="1" min="35" max="35"/>
+    <col width="25" customWidth="1" min="36" max="36"/>
+    <col width="20" customWidth="1" min="37" max="37"/>
+    <col width="23" customWidth="1" min="38" max="38"/>
+    <col width="23" customWidth="1" min="39" max="39"/>
+    <col width="2" customWidth="1" min="40" max="40"/>
+    <col width="19" customWidth="1" min="41" max="41"/>
+    <col width="20" customWidth="1" min="42" max="42"/>
+    <col width="27" customWidth="1" min="43" max="43"/>
+    <col width="2" customWidth="1" min="44" max="44"/>
+    <col width="20" customWidth="1" min="45" max="45"/>
+    <col width="21" customWidth="1" min="46" max="46"/>
+    <col width="28" customWidth="1" min="47" max="47"/>
+    <col width="2" customWidth="1" min="48" max="48"/>
+    <col width="20" customWidth="1" min="49" max="49"/>
+    <col width="21" customWidth="1" min="50" max="50"/>
+    <col width="20" customWidth="1" min="51" max="51"/>
+    <col width="28" customWidth="1" min="52" max="52"/>
+    <col width="2" customWidth="1" min="53" max="53"/>
+    <col width="9" customWidth="1" min="54" max="54"/>
+    <col width="17" customWidth="1" min="55" max="55"/>
+    <col width="24" customWidth="1" min="56" max="56"/>
+    <col width="16" customWidth="1" min="57" max="57"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Student ID</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Course/Section</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>LRN</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Surname</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Firstname</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Middle Initial</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Gender</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Age</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Birthdate</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Birthplace</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Nationality</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Religion</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Marital Status</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Language Spoken</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>Street</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>Barangay</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>City</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>Zip Code</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>Province</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>Country</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>Contact Number</t>
+        </is>
+      </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>Father's Name</t>
+        </is>
+      </c>
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
+          <t>Father's Occupation</t>
+        </is>
+      </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>Father's Contact No</t>
+        </is>
+      </c>
+      <c r="AE1" s="1" t="inlineStr">
+        <is>
+          <t>Mother's Name</t>
+        </is>
+      </c>
+      <c r="AF1" s="1" t="inlineStr">
+        <is>
+          <t>Mother's Occupation</t>
+        </is>
+      </c>
+      <c r="AG1" s="1" t="inlineStr">
+        <is>
+          <t>Mother's Contact No</t>
+        </is>
+      </c>
+      <c r="AI1" s="1" t="inlineStr">
+        <is>
+          <t>Guardian's Name</t>
+        </is>
+      </c>
+      <c r="AJ1" s="1" t="inlineStr">
+        <is>
+          <t>Guardian's Relationship</t>
+        </is>
+      </c>
+      <c r="AK1" s="1" t="inlineStr">
+        <is>
+          <t>Guardian's Address</t>
+        </is>
+      </c>
+      <c r="AL1" s="1" t="inlineStr">
+        <is>
+          <t>Guardian's Occupation</t>
+        </is>
+      </c>
+      <c r="AM1" s="1" t="inlineStr">
+        <is>
+          <t>Guardian's Contact No</t>
+        </is>
+      </c>
+      <c r="AO1" s="1" t="inlineStr">
+        <is>
+          <t>Elementary School</t>
+        </is>
+      </c>
+      <c r="AP1" s="1" t="inlineStr">
+        <is>
+          <t>Elementary Address</t>
+        </is>
+      </c>
+      <c r="AQ1" s="1" t="inlineStr">
+        <is>
+          <t>Elementary Year Graduated</t>
+        </is>
+      </c>
+      <c r="AS1" s="1" t="inlineStr">
+        <is>
+          <t>Junior High School</t>
+        </is>
+      </c>
+      <c r="AT1" s="1" t="inlineStr">
+        <is>
+          <t>Junior High Address</t>
+        </is>
+      </c>
+      <c r="AU1" s="1" t="inlineStr">
+        <is>
+          <t>Junior High Year Graduated</t>
+        </is>
+      </c>
+      <c r="AW1" s="1" t="inlineStr">
+        <is>
+          <t>Senior High School</t>
+        </is>
+      </c>
+      <c r="AX1" s="1" t="inlineStr">
+        <is>
+          <t>Senior High Address</t>
+        </is>
+      </c>
+      <c r="AY1" s="1" t="inlineStr">
+        <is>
+          <t>Senior High Strand</t>
+        </is>
+      </c>
+      <c r="AZ1" s="1" t="inlineStr">
+        <is>
+          <t>Senior High Year Graduated</t>
+        </is>
+      </c>
+      <c r="BB1" s="1" t="inlineStr">
+        <is>
+          <t>College</t>
+        </is>
+      </c>
+      <c r="BC1" s="1" t="inlineStr">
+        <is>
+          <t>College Address</t>
+        </is>
+      </c>
+      <c r="BD1" s="1" t="inlineStr">
+        <is>
+          <t>College Year Graduated</t>
+        </is>
+      </c>
+      <c r="BE1" s="1" t="inlineStr">
+        <is>
+          <t>Student Status</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>123123</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>1B</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>123123</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>jok</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>jok</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>wce</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>32</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>June 14, 1932</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>awec</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>awerc</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>Born Again</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>Single</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>awerc</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>awerc</t>
+        </is>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>awerc</t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>awerc</t>
+        </is>
+      </c>
+      <c r="U2" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="V2" t="inlineStr">
+        <is>
+          <t>awerc</t>
+        </is>
+      </c>
+      <c r="W2" t="inlineStr">
+        <is>
+          <t>awerc</t>
+        </is>
+      </c>
+      <c r="Y2" t="inlineStr">
+        <is>
+          <t>jok@gmail.com</t>
+        </is>
+      </c>
+      <c r="Z2" t="inlineStr">
+        <is>
+          <t>123123</t>
+        </is>
+      </c>
+      <c r="AB2" t="inlineStr">
+        <is>
+          <t>awdewa</t>
+        </is>
+      </c>
+      <c r="AC2" t="inlineStr">
+        <is>
+          <t>awdawd</t>
+        </is>
+      </c>
+      <c r="AD2" t="inlineStr">
+        <is>
+          <t>123123</t>
+        </is>
+      </c>
+      <c r="AE2" t="inlineStr">
+        <is>
+          <t>awdawd</t>
+        </is>
+      </c>
+      <c r="AF2" t="inlineStr">
+        <is>
+          <t>awdawd</t>
+        </is>
+      </c>
+      <c r="AG2" t="inlineStr">
+        <is>
+          <t>123123</t>
+        </is>
+      </c>
+      <c r="AO2" t="inlineStr">
+        <is>
+          <t>we</t>
+        </is>
+      </c>
+      <c r="AP2" t="inlineStr">
+        <is>
+          <t>waef</t>
+        </is>
+      </c>
+      <c r="AQ2" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="AS2" t="inlineStr">
+        <is>
+          <t>awef</t>
+        </is>
+      </c>
+      <c r="AT2" t="inlineStr">
+        <is>
+          <t>awef</t>
+        </is>
+      </c>
+      <c r="AU2" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="AW2" t="inlineStr">
+        <is>
+          <t>waef</t>
+        </is>
+      </c>
+      <c r="AX2" t="inlineStr">
+        <is>
+          <t>awef</t>
+        </is>
+      </c>
+      <c r="AY2" t="inlineStr">
+        <is>
+          <t>awef</t>
+        </is>
+      </c>
+      <c r="AZ2" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="BB2" t="inlineStr">
+        <is>
+          <t>awef</t>
+        </is>
+      </c>
+      <c r="BC2" t="inlineStr">
+        <is>
+          <t>awef</t>
+        </is>
+      </c>
+      <c r="BD2" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="BE2" t="inlineStr">
+        <is>
+          <t>Old Student</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
created a working updating function
</commit_message>
<xml_diff>
--- a/user_account_data.xlsx
+++ b/user_account_data.xlsx
@@ -418,7 +418,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -487,6 +487,33 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>admin@gmail.com</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>admin123</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -498,7 +525,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BH2"/>
+  <dimension ref="A1:BH3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -512,34 +539,34 @@
     <col width="2" customWidth="1" min="4" max="4"/>
     <col width="9" customWidth="1" min="5" max="5"/>
     <col width="12" customWidth="1" min="6" max="6"/>
-    <col width="16" customWidth="1" min="7" max="7"/>
+    <col width="20" customWidth="1" min="7" max="7"/>
     <col width="2" customWidth="1" min="8" max="8"/>
     <col width="8" customWidth="1" min="9" max="9"/>
     <col width="5" customWidth="1" min="10" max="10"/>
-    <col width="15" customWidth="1" min="11" max="11"/>
+    <col width="17" customWidth="1" min="11" max="11"/>
     <col width="14" customWidth="1" min="12" max="12"/>
-    <col width="14" customWidth="1" min="13" max="13"/>
+    <col width="20" customWidth="1" min="13" max="13"/>
     <col width="12" customWidth="1" min="14" max="14"/>
     <col width="16" customWidth="1" min="15" max="15"/>
-    <col width="17" customWidth="1" min="16" max="16"/>
+    <col width="20" customWidth="1" min="16" max="16"/>
     <col width="2" customWidth="1" min="17" max="17"/>
     <col width="12" customWidth="1" min="18" max="18"/>
     <col width="12" customWidth="1" min="19" max="19"/>
-    <col width="14" customWidth="1" min="20" max="20"/>
+    <col width="20" customWidth="1" min="20" max="20"/>
     <col width="11" customWidth="1" min="21" max="21"/>
-    <col width="13" customWidth="1" min="22" max="22"/>
-    <col width="11" customWidth="1" min="23" max="23"/>
+    <col width="20" customWidth="1" min="22" max="22"/>
+    <col width="20" customWidth="1" min="23" max="23"/>
     <col width="2" customWidth="1" min="24" max="24"/>
     <col width="16" customWidth="1" min="25" max="25"/>
     <col width="16" customWidth="1" min="26" max="26"/>
     <col width="2" customWidth="1" min="27" max="27"/>
-    <col width="16" customWidth="1" min="28" max="28"/>
-    <col width="18" customWidth="1" min="29" max="29"/>
+    <col width="20" customWidth="1" min="28" max="28"/>
+    <col width="20" customWidth="1" min="29" max="29"/>
     <col width="21" customWidth="1" min="30" max="30"/>
     <col width="21" customWidth="1" min="31" max="31"/>
     <col width="2" customWidth="1" min="32" max="32"/>
-    <col width="15" customWidth="1" min="33" max="33"/>
-    <col width="18" customWidth="1" min="34" max="34"/>
+    <col width="20" customWidth="1" min="33" max="33"/>
+    <col width="20" customWidth="1" min="34" max="34"/>
     <col width="21" customWidth="1" min="35" max="35"/>
     <col width="21" customWidth="1" min="36" max="36"/>
     <col width="2" customWidth="1" min="37" max="37"/>
@@ -562,8 +589,8 @@
     <col width="20" customWidth="1" min="54" max="54"/>
     <col width="28" customWidth="1" min="55" max="55"/>
     <col width="2" customWidth="1" min="56" max="56"/>
-    <col width="16" customWidth="1" min="57" max="57"/>
-    <col width="17" customWidth="1" min="58" max="58"/>
+    <col width="20" customWidth="1" min="57" max="57"/>
+    <col width="20" customWidth="1" min="58" max="58"/>
     <col width="24" customWidth="1" min="59" max="59"/>
     <col width="16" customWidth="1" min="60" max="60"/>
   </cols>
@@ -843,22 +870,22 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>aaaaaaa</t>
+          <t>bbbbbbbbbbbbbbbbbbb</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Male</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>31</t>
+          <t>32</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>June 23, 2026</t>
+          <t>September 25, 1909</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
@@ -868,195 +895,392 @@
       </c>
       <c r="M2" t="inlineStr">
         <is>
+          <t>bbbbbbbbbbbbbbbbbbb</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>Iglesia ni Cristo</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>Single</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>bbbbbbbbbbbbbbbbbbb</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>aaaaaaaaaa</t>
+        </is>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>bbbbbbbbbbbbbbbbbbb</t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>bbbbbbbbbbbbbbbbbbb</t>
+        </is>
+      </c>
+      <c r="U2" t="inlineStr">
+        <is>
+          <t>123456789</t>
+        </is>
+      </c>
+      <c r="V2" t="inlineStr">
+        <is>
+          <t>aaaaaaaaaaa</t>
+        </is>
+      </c>
+      <c r="W2" t="inlineStr">
+        <is>
+          <t>bbbbbbbbbbbbbbbbbbb</t>
+        </is>
+      </c>
+      <c r="Y2" t="inlineStr">
+        <is>
+          <t>test@gmail.com</t>
+        </is>
+      </c>
+      <c r="Z2" t="inlineStr">
+        <is>
+          <t>123456789</t>
+        </is>
+      </c>
+      <c r="AB2" t="inlineStr">
+        <is>
+          <t>aaaaaaaaaaaaaa</t>
+        </is>
+      </c>
+      <c r="AC2" t="inlineStr">
+        <is>
+          <t>bbbbbbbbbbbbbbbbbbb</t>
+        </is>
+      </c>
+      <c r="AD2" t="inlineStr">
+        <is>
+          <t>aaaaaaaaaaaaa</t>
+        </is>
+      </c>
+      <c r="AE2" t="inlineStr">
+        <is>
+          <t>123456789</t>
+        </is>
+      </c>
+      <c r="AG2" t="inlineStr">
+        <is>
+          <t>aaaaaaaaaaaaa</t>
+        </is>
+      </c>
+      <c r="AH2" t="inlineStr">
+        <is>
+          <t>aaaaaaaaaaaaaaa</t>
+        </is>
+      </c>
+      <c r="AI2" t="inlineStr">
+        <is>
+          <t>aabbbbbbbbbbbbbbbbbbb</t>
+        </is>
+      </c>
+      <c r="AJ2" t="inlineStr">
+        <is>
+          <t>123456789</t>
+        </is>
+      </c>
+      <c r="AR2" t="inlineStr">
+        <is>
+          <t>bbbbbbbbbbbbbbbbbbb</t>
+        </is>
+      </c>
+      <c r="AS2" t="inlineStr">
+        <is>
+          <t>aaaaaaaa</t>
+        </is>
+      </c>
+      <c r="AT2" t="inlineStr">
+        <is>
+          <t>123456789</t>
+        </is>
+      </c>
+      <c r="AV2" t="inlineStr">
+        <is>
+          <t>aaaaaaaaaaaaaa</t>
+        </is>
+      </c>
+      <c r="AW2" t="inlineStr">
+        <is>
+          <t>bbbbbbbbbbbbbbbbbbb</t>
+        </is>
+      </c>
+      <c r="AX2" t="inlineStr">
+        <is>
+          <t>123456789</t>
+        </is>
+      </c>
+      <c r="AZ2" t="inlineStr">
+        <is>
+          <t>aaaaaaaaaaaaaa</t>
+        </is>
+      </c>
+      <c r="BA2" t="inlineStr">
+        <is>
+          <t>aaaaaaaaaaaaaa</t>
+        </is>
+      </c>
+      <c r="BB2" t="inlineStr">
+        <is>
+          <t>aaaaaaaaaaaaaa</t>
+        </is>
+      </c>
+      <c r="BC2" t="inlineStr">
+        <is>
+          <t>123456789</t>
+        </is>
+      </c>
+      <c r="BE2" t="inlineStr">
+        <is>
+          <t>bbbbbbbbbbbbbbbbbbb</t>
+        </is>
+      </c>
+      <c r="BF2" t="inlineStr">
+        <is>
+          <t>bbbbbbbbbbbbbbbbbbb</t>
+        </is>
+      </c>
+      <c r="BG2" t="inlineStr">
+        <is>
+          <t>123456789</t>
+        </is>
+      </c>
+      <c r="BH2" t="inlineStr">
+        <is>
+          <t>New Student</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>123456789</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>1A</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>123456789</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>awefawe</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>awfeawefwe</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>bbbbbbbbbbbbbbbbbb</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>August 23, 1936</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
           <t>aaaaaaaaaaaa</t>
         </is>
       </c>
-      <c r="N2" t="inlineStr">
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>bbbbbbbbbbbbbbbbbb</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
         <is>
           <t>Born Again</t>
         </is>
       </c>
-      <c r="O2" t="inlineStr">
+      <c r="O3" t="inlineStr">
         <is>
           <t>Single</t>
         </is>
       </c>
-      <c r="P2" t="inlineStr">
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>bbbbbbbbbbbbbbbbbb</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>aaaaaaaaaa</t>
+        </is>
+      </c>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>aaaaaaaaaa</t>
+        </is>
+      </c>
+      <c r="T3" t="inlineStr">
+        <is>
+          <t>bbbbbbbbbbbbbbbbbb</t>
+        </is>
+      </c>
+      <c r="U3" t="inlineStr">
+        <is>
+          <t>123456789</t>
+        </is>
+      </c>
+      <c r="V3" t="inlineStr">
+        <is>
+          <t>bbbbbbbbbbbbbbbbbb</t>
+        </is>
+      </c>
+      <c r="W3" t="inlineStr">
+        <is>
+          <t>bbbbbbbbbbbbbbbbbb</t>
+        </is>
+      </c>
+      <c r="Y3" t="inlineStr">
+        <is>
+          <t>test@gmail.com</t>
+        </is>
+      </c>
+      <c r="Z3" t="inlineStr">
+        <is>
+          <t>123456789</t>
+        </is>
+      </c>
+      <c r="AB3" t="inlineStr">
+        <is>
+          <t>bbbbbbbbbbbbbbbbbb</t>
+        </is>
+      </c>
+      <c r="AC3" t="inlineStr">
+        <is>
+          <t>bbbbbbbbbbbbbbbbbb</t>
+        </is>
+      </c>
+      <c r="AD3" t="inlineStr">
+        <is>
+          <t>aaaaaaaaaaaaa</t>
+        </is>
+      </c>
+      <c r="AE3" t="inlineStr">
+        <is>
+          <t>123456789</t>
+        </is>
+      </c>
+      <c r="AG3" t="inlineStr">
+        <is>
+          <t>bbbbbbbbbbbbbbbbbb</t>
+        </is>
+      </c>
+      <c r="AH3" t="inlineStr">
+        <is>
+          <t>bbbbbbbbbbbbbbbbbb</t>
+        </is>
+      </c>
+      <c r="AI3" t="inlineStr">
+        <is>
+          <t>aaaaaaaaaaaaa</t>
+        </is>
+      </c>
+      <c r="AJ3" t="inlineStr">
+        <is>
+          <t>123456789</t>
+        </is>
+      </c>
+      <c r="AR3" t="inlineStr">
         <is>
           <t>aaaaaaaaaaaaaa</t>
         </is>
       </c>
-      <c r="R2" t="inlineStr">
-        <is>
-          <t>aaaaaaaaaa</t>
-        </is>
-      </c>
-      <c r="S2" t="inlineStr">
-        <is>
-          <t>aaaaaaaaaa</t>
-        </is>
-      </c>
-      <c r="T2" t="inlineStr">
-        <is>
-          <t>aaaaaaaaaaaa</t>
-        </is>
-      </c>
-      <c r="U2" t="inlineStr">
-        <is>
-          <t>123456789</t>
-        </is>
-      </c>
-      <c r="V2" t="inlineStr">
-        <is>
-          <t>aaaaaaaaaaa</t>
-        </is>
-      </c>
-      <c r="W2" t="inlineStr">
-        <is>
-          <t>aaaaaaaaa</t>
-        </is>
-      </c>
-      <c r="Y2" t="inlineStr">
-        <is>
-          <t>test@gmail.com</t>
-        </is>
-      </c>
-      <c r="Z2" t="inlineStr">
-        <is>
-          <t>123456789</t>
-        </is>
-      </c>
-      <c r="AB2" t="inlineStr">
+      <c r="AS3" t="inlineStr">
+        <is>
+          <t>aaaaaaaa</t>
+        </is>
+      </c>
+      <c r="AT3" t="inlineStr">
+        <is>
+          <t>123456789</t>
+        </is>
+      </c>
+      <c r="AV3" t="inlineStr">
+        <is>
+          <t>bbbbbbbbbbbbbbbbbb</t>
+        </is>
+      </c>
+      <c r="AW3" t="inlineStr">
+        <is>
+          <t>bbbbbbbbbbbbbbbbbb</t>
+        </is>
+      </c>
+      <c r="AX3" t="inlineStr">
+        <is>
+          <t>123456789</t>
+        </is>
+      </c>
+      <c r="AZ3" t="inlineStr">
         <is>
           <t>aaaaaaaaaaaaaa</t>
         </is>
       </c>
-      <c r="AC2" t="inlineStr">
+      <c r="BA3" t="inlineStr">
         <is>
           <t>aaaaaaaaaaaaaa</t>
         </is>
       </c>
-      <c r="AD2" t="inlineStr">
-        <is>
-          <t>aaaaaaaaaaaaa</t>
-        </is>
-      </c>
-      <c r="AE2" t="inlineStr">
-        <is>
-          <t>123456789</t>
-        </is>
-      </c>
-      <c r="AG2" t="inlineStr">
-        <is>
-          <t>aaaaaaaaaaaaa</t>
-        </is>
-      </c>
-      <c r="AH2" t="inlineStr">
-        <is>
-          <t>aaaaaaaaaaaaaaa</t>
-        </is>
-      </c>
-      <c r="AI2" t="inlineStr">
-        <is>
-          <t>aaaaaaaaaaaaa</t>
-        </is>
-      </c>
-      <c r="AJ2" t="inlineStr">
-        <is>
-          <t>123456789</t>
-        </is>
-      </c>
-      <c r="AL2" t="inlineStr">
-        <is>
-          <t>aaaaaaaaaaaaaaa</t>
-        </is>
-      </c>
-      <c r="AM2" t="inlineStr">
-        <is>
-          <t>aaaaaaaaaaaaa</t>
-        </is>
-      </c>
-      <c r="AN2" t="inlineStr">
-        <is>
-          <t>aaaaaaaaaaaaa</t>
-        </is>
-      </c>
-      <c r="AO2" t="inlineStr">
-        <is>
-          <t>aaaaaaaaaaaaa</t>
-        </is>
-      </c>
-      <c r="AP2" t="inlineStr">
-        <is>
-          <t>123456789</t>
-        </is>
-      </c>
-      <c r="AR2" t="inlineStr">
+      <c r="BB3" t="inlineStr">
         <is>
           <t>aaaaaaaaaaaaaa</t>
         </is>
       </c>
-      <c r="AS2" t="inlineStr">
-        <is>
-          <t>aaaaaaaa</t>
-        </is>
-      </c>
-      <c r="AT2" t="inlineStr">
-        <is>
-          <t>123456789</t>
-        </is>
-      </c>
-      <c r="AV2" t="inlineStr">
-        <is>
-          <t>aaaaaaaaaaaaaa</t>
-        </is>
-      </c>
-      <c r="AW2" t="inlineStr">
-        <is>
-          <t>aaaaaaaaaaaaaa</t>
-        </is>
-      </c>
-      <c r="AX2" t="inlineStr">
-        <is>
-          <t>123456789</t>
-        </is>
-      </c>
-      <c r="AZ2" t="inlineStr">
-        <is>
-          <t>aaaaaaaaaaaaaa</t>
-        </is>
-      </c>
-      <c r="BA2" t="inlineStr">
-        <is>
-          <t>aaaaaaaaaaaaaa</t>
-        </is>
-      </c>
-      <c r="BB2" t="inlineStr">
-        <is>
-          <t>aaaaaaaaaaaaaa</t>
-        </is>
-      </c>
-      <c r="BC2" t="inlineStr">
-        <is>
-          <t>123456789</t>
-        </is>
-      </c>
-      <c r="BE2" t="inlineStr">
-        <is>
-          <t>aaaaaaaaaaaaaa</t>
-        </is>
-      </c>
-      <c r="BF2" t="inlineStr">
-        <is>
-          <t>aaaaaaaaaaaaaa</t>
-        </is>
-      </c>
-      <c r="BG2" t="inlineStr">
-        <is>
-          <t>123456789</t>
-        </is>
-      </c>
-      <c r="BH2" t="inlineStr">
+      <c r="BC3" t="inlineStr">
+        <is>
+          <t>123456789</t>
+        </is>
+      </c>
+      <c r="BE3" t="inlineStr">
+        <is>
+          <t>bbbbbbbbbbbbbbbbbb</t>
+        </is>
+      </c>
+      <c r="BF3" t="inlineStr">
+        <is>
+          <t>bbbbbbbbbbbbbbbbbb</t>
+        </is>
+      </c>
+      <c r="BG3" t="inlineStr">
+        <is>
+          <t>123456789</t>
+        </is>
+      </c>
+      <c r="BH3" t="inlineStr">
         <is>
           <t>New Student</t>
         </is>

</xml_diff>